<commit_message>
Delete unnecessary diagram files
</commit_message>
<xml_diff>
--- a/Documentation/Project Overview.xlsx
+++ b/Documentation/Project Overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Working Space\Mobile Project - Ship Journal\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Working Space\Ship-Journal\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C48AC3-299C-46ED-939A-663587EC7D52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED2D85A-DD32-440A-80FD-47DC7EE050F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="4" xr2:uid="{A0F38D15-187F-4603-A4E4-C66A63208D0B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="2" xr2:uid="{A0F38D15-187F-4603-A4E4-C66A63208D0B}"/>
   </bookViews>
   <sheets>
     <sheet name=" Revision History" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
   <si>
     <t>Version</t>
   </si>
@@ -214,6 +214,10 @@
   </si>
   <si>
     <t>Character</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Insert the logo of the National Research and Development Agency, Fisheries Research and Education Agency, in the top right corner of the first level</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -9655,8 +9659,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="26207357" y="1211036"/>
-          <a:ext cx="3533735" cy="6383027"/>
+          <a:off x="26289000" y="1187824"/>
+          <a:ext cx="3549743" cy="6206934"/>
           <a:chOff x="8189026" y="682665"/>
           <a:chExt cx="3183247" cy="3803567"/>
         </a:xfrm>
@@ -10128,8 +10132,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="20764500" y="1211984"/>
-          <a:ext cx="3533735" cy="6382078"/>
+          <a:off x="20820529" y="1188772"/>
+          <a:ext cx="3549744" cy="6205985"/>
           <a:chOff x="18340779" y="725723"/>
           <a:chExt cx="3183248" cy="3806675"/>
         </a:xfrm>
@@ -10794,8 +10798,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="47218283" y="8037736"/>
-          <a:ext cx="3634521" cy="5148291"/>
+          <a:off x="47398378" y="7819221"/>
+          <a:ext cx="3653731" cy="4946585"/>
           <a:chOff x="27944990" y="737920"/>
           <a:chExt cx="3196481" cy="3898206"/>
         </a:xfrm>
@@ -12373,8 +12377,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="42718326" y="8049164"/>
-          <a:ext cx="3539079" cy="5130564"/>
+          <a:off x="42879211" y="7830649"/>
+          <a:ext cx="3555087" cy="4928858"/>
           <a:chOff x="27963633" y="5221724"/>
           <a:chExt cx="3181788" cy="3896347"/>
         </a:xfrm>
@@ -13821,8 +13825,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="15328786" y="1229673"/>
-          <a:ext cx="3530552" cy="6440106"/>
+          <a:off x="15359202" y="1206461"/>
+          <a:ext cx="3546560" cy="6254409"/>
           <a:chOff x="13431899" y="760845"/>
           <a:chExt cx="3156281" cy="3890158"/>
         </a:xfrm>
@@ -14152,7 +14156,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="15689283" y="4141065"/>
+            <a:off x="15689283" y="4108187"/>
             <a:ext cx="698852" cy="322393"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -14448,8 +14452,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31691105" y="14360368"/>
-          <a:ext cx="3597886" cy="5152697"/>
+          <a:off x="31798362" y="13892122"/>
+          <a:ext cx="3616295" cy="4950991"/>
           <a:chOff x="27998557" y="14473052"/>
           <a:chExt cx="3240382" cy="3893177"/>
         </a:xfrm>
@@ -16349,8 +16353,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="42675167" y="1213999"/>
-          <a:ext cx="3561219" cy="6457752"/>
+          <a:off x="42836052" y="1190787"/>
+          <a:ext cx="3577227" cy="6272055"/>
           <a:chOff x="37652894" y="695690"/>
           <a:chExt cx="3186940" cy="3641610"/>
         </a:xfrm>
@@ -18083,8 +18087,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="47207422" y="1211036"/>
-          <a:ext cx="3641795" cy="6460933"/>
+          <a:off x="47387517" y="1187824"/>
+          <a:ext cx="3661005" cy="6275236"/>
           <a:chOff x="37652894" y="695690"/>
           <a:chExt cx="3190115" cy="3644785"/>
         </a:xfrm>
@@ -19812,8 +19816,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="52047321" y="1211036"/>
-          <a:ext cx="3564400" cy="6457758"/>
+          <a:off x="52253029" y="1187824"/>
+          <a:ext cx="3580409" cy="6272061"/>
           <a:chOff x="37652894" y="695690"/>
           <a:chExt cx="3190115" cy="3644785"/>
         </a:xfrm>
@@ -21541,8 +21545,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="56809821" y="1211036"/>
-          <a:ext cx="3561225" cy="6460933"/>
+          <a:off x="57037941" y="1187824"/>
+          <a:ext cx="3577233" cy="6275236"/>
           <a:chOff x="37652894" y="695690"/>
           <a:chExt cx="3190115" cy="3644785"/>
         </a:xfrm>
@@ -23670,8 +23674,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="62679413" y="1231529"/>
-          <a:ext cx="3535987" cy="6457758"/>
+          <a:off x="62933146" y="1208317"/>
+          <a:ext cx="3551996" cy="6272061"/>
           <a:chOff x="59141720" y="969818"/>
           <a:chExt cx="3164884" cy="3644791"/>
         </a:xfrm>
@@ -27152,8 +27156,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9936513" y="1107661"/>
-          <a:ext cx="3533734" cy="6569654"/>
+          <a:off x="9941315" y="1094054"/>
+          <a:ext cx="3549743" cy="6374352"/>
           <a:chOff x="8657441" y="675408"/>
           <a:chExt cx="3193556" cy="3763407"/>
         </a:xfrm>
@@ -28054,8 +28058,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31695067" y="26094525"/>
-          <a:ext cx="3504224" cy="5137317"/>
+          <a:off x="31802324" y="25165237"/>
+          <a:ext cx="3522633" cy="4935612"/>
           <a:chOff x="27945820" y="22949647"/>
           <a:chExt cx="3141633" cy="3755818"/>
         </a:xfrm>
@@ -28803,8 +28807,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31656564" y="8440431"/>
-          <a:ext cx="3525913" cy="5139173"/>
+          <a:off x="31763821" y="8202706"/>
+          <a:ext cx="3544322" cy="4937467"/>
           <a:chOff x="27936265" y="9681882"/>
           <a:chExt cx="3176022" cy="3757675"/>
         </a:xfrm>
@@ -29658,8 +29662,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31714027" y="1241054"/>
-          <a:ext cx="3521497" cy="6467283"/>
+          <a:off x="31821284" y="1217842"/>
+          <a:ext cx="3539906" cy="6281586"/>
           <a:chOff x="46386774" y="6092825"/>
           <a:chExt cx="3184493" cy="3811623"/>
         </a:xfrm>
@@ -31026,8 +31030,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31678989" y="20163600"/>
-          <a:ext cx="3588341" cy="5139073"/>
+          <a:off x="31786246" y="19464833"/>
+          <a:ext cx="3606750" cy="4937367"/>
           <a:chOff x="27961865" y="13634599"/>
           <a:chExt cx="3228925" cy="3767099"/>
         </a:xfrm>
@@ -32671,7 +32675,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="15633011" y="953294"/>
-          <a:ext cx="3524363" cy="5421680"/>
+          <a:ext cx="3524363" cy="6161268"/>
           <a:chOff x="13590364" y="26574050"/>
           <a:chExt cx="3202194" cy="4011233"/>
         </a:xfrm>
@@ -33318,7 +33322,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="21083782" y="948551"/>
-          <a:ext cx="3502949" cy="5286994"/>
+          <a:ext cx="3502949" cy="6026582"/>
           <a:chOff x="13435075" y="760845"/>
           <a:chExt cx="3153104" cy="3890158"/>
         </a:xfrm>
@@ -33865,7 +33869,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>printing</a:t>
+            <a:t>Printing</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -34101,7 +34105,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="26505064" y="941666"/>
-          <a:ext cx="3554644" cy="5358267"/>
+          <a:ext cx="3554644" cy="6097855"/>
           <a:chOff x="18406733" y="715323"/>
           <a:chExt cx="3195282" cy="3708174"/>
         </a:xfrm>
@@ -34475,7 +34479,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="26510983" y="6763091"/>
+          <a:off x="26510983" y="7502679"/>
           <a:ext cx="3551469" cy="4941573"/>
           <a:chOff x="18406733" y="715323"/>
           <a:chExt cx="3195282" cy="3708174"/>
@@ -35056,7 +35060,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="21095353" y="6824103"/>
+          <a:off x="21095353" y="7563691"/>
           <a:ext cx="3502949" cy="4818215"/>
           <a:chOff x="13435075" y="760845"/>
           <a:chExt cx="3153104" cy="3890158"/>
@@ -35499,7 +35503,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="10151794" y="913790"/>
-          <a:ext cx="3538981" cy="5459735"/>
+          <a:ext cx="3538981" cy="6199323"/>
           <a:chOff x="8657441" y="675408"/>
           <a:chExt cx="3193556" cy="3763407"/>
         </a:xfrm>
@@ -41409,7 +41413,7 @@
   <dimension ref="F2:AH3"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD25" sqref="AD25"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="20.25" x14ac:dyDescent="0.35"/>
@@ -41476,8 +41480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E4BCCA-608F-4C56-8910-30F772A13230}">
   <dimension ref="B2:AM106"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="U43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -41568,7 +41572,7 @@
         <v>31</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="D7" s="13">
         <v>45567</v>
@@ -41680,7 +41684,7 @@
   <dimension ref="B2:AM17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -41766,7 +41770,7 @@
         <v>45567</v>
       </c>
     </row>
-    <row r="7" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:39" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B7" s="10" t="s">
         <v>52</v>
       </c>
@@ -41777,7 +41781,7 @@
         <v>45567</v>
       </c>
     </row>
-    <row r="8" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:39" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B8" s="10" t="s">
         <v>33</v>
       </c>
@@ -41788,7 +41792,7 @@
         <v>45568</v>
       </c>
     </row>
-    <row r="9" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:39" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B9" s="10" t="s">
         <v>35</v>
       </c>
@@ -41868,7 +41872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65059E32-4F8B-40EB-A291-F3015047563B}">
   <dimension ref="B2:AM17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update exported screen design and icon files
</commit_message>
<xml_diff>
--- a/Documentation/Project Overview.xlsx
+++ b/Documentation/Project Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Working Space\Ship-Journal\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED2D85A-DD32-440A-80FD-47DC7EE050F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7F8BE2-1B02-478C-8123-83F7707FE960}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="2" xr2:uid="{A0F38D15-187F-4603-A4E4-C66A63208D0B}"/>
   </bookViews>
@@ -9659,8 +9659,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="26289000" y="1187824"/>
-          <a:ext cx="3549743" cy="6206934"/>
+          <a:off x="26355675" y="1190625"/>
+          <a:ext cx="3560949" cy="6255120"/>
           <a:chOff x="8189026" y="682665"/>
           <a:chExt cx="3183247" cy="3803567"/>
         </a:xfrm>
@@ -10132,8 +10132,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="20820529" y="1188772"/>
-          <a:ext cx="3549744" cy="6205985"/>
+          <a:off x="20869275" y="1191573"/>
+          <a:ext cx="3560949" cy="6254171"/>
           <a:chOff x="18340779" y="725723"/>
           <a:chExt cx="3183248" cy="3806675"/>
         </a:xfrm>
@@ -10798,8 +10798,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="47398378" y="7819221"/>
-          <a:ext cx="3653731" cy="4946585"/>
+          <a:off x="47524444" y="7875811"/>
+          <a:ext cx="3667178" cy="5005416"/>
           <a:chOff x="27944990" y="737920"/>
           <a:chExt cx="3196481" cy="3898206"/>
         </a:xfrm>
@@ -12377,8 +12377,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="42879211" y="7830649"/>
-          <a:ext cx="3555087" cy="4928858"/>
+          <a:off x="42991830" y="7887239"/>
+          <a:ext cx="3566293" cy="4987689"/>
           <a:chOff x="27963633" y="5221724"/>
           <a:chExt cx="3181788" cy="3896347"/>
         </a:xfrm>
@@ -13825,8 +13825,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="15359202" y="1206461"/>
-          <a:ext cx="3546560" cy="6254409"/>
+          <a:off x="15390018" y="1209262"/>
+          <a:ext cx="3557766" cy="6305396"/>
           <a:chOff x="13431899" y="760845"/>
           <a:chExt cx="3156281" cy="3890158"/>
         </a:xfrm>
@@ -14452,8 +14452,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31798362" y="13892122"/>
-          <a:ext cx="3616295" cy="4950991"/>
+          <a:off x="31882966" y="14021550"/>
+          <a:ext cx="3619657" cy="5009822"/>
           <a:chOff x="27998557" y="14473052"/>
           <a:chExt cx="3240382" cy="3893177"/>
         </a:xfrm>
@@ -16200,16 +16200,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>50</xdr:col>
-      <xdr:colOff>618968</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>241193</xdr:rowOff>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>81087</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>185164</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>57</xdr:col>
-      <xdr:colOff>167292</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>14652</xdr:rowOff>
+      <xdr:colOff>312969</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>193947</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -16224,8 +16224,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="40595393" y="10128143"/>
-          <a:ext cx="4348924" cy="725959"/>
+          <a:off x="40713616" y="11637576"/>
+          <a:ext cx="4333235" cy="714753"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -16353,8 +16353,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="42836052" y="1190787"/>
-          <a:ext cx="3577227" cy="6272055"/>
+          <a:off x="42948671" y="1193588"/>
+          <a:ext cx="3588433" cy="6323042"/>
           <a:chOff x="37652894" y="695690"/>
           <a:chExt cx="3186940" cy="3641610"/>
         </a:xfrm>
@@ -17460,8 +17460,8 @@
                 <a:p>
                   <a:pPr algn="ctr"/>
                   <a:r>
-                    <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
-                    <a:t>項目</a:t>
+                    <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
+                    <a:t>Item</a:t>
                   </a:r>
                   <a:endParaRPr lang="en-US" sz="1100" b="1"/>
                 </a:p>
@@ -17511,8 +17511,8 @@
                 <a:p>
                   <a:pPr algn="ctr"/>
                   <a:r>
-                    <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
-                    <a:t>数値</a:t>
+                    <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
+                    <a:t>Qty</a:t>
                   </a:r>
                   <a:endParaRPr lang="en-US" sz="1100" b="1"/>
                 </a:p>
@@ -18087,8 +18087,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="47387517" y="1187824"/>
-          <a:ext cx="3661005" cy="6275236"/>
+          <a:off x="47513583" y="1190625"/>
+          <a:ext cx="3674452" cy="6326223"/>
           <a:chOff x="37652894" y="695690"/>
           <a:chExt cx="3190115" cy="3644785"/>
         </a:xfrm>
@@ -19816,8 +19816,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="52253029" y="1187824"/>
-          <a:ext cx="3580409" cy="6272061"/>
+          <a:off x="52397025" y="1190625"/>
+          <a:ext cx="3591614" cy="6323048"/>
           <a:chOff x="37652894" y="695690"/>
           <a:chExt cx="3190115" cy="3644785"/>
         </a:xfrm>
@@ -21545,8 +21545,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="57037941" y="1187824"/>
-          <a:ext cx="3577233" cy="6275236"/>
+          <a:off x="57197625" y="1190625"/>
+          <a:ext cx="3588439" cy="6326223"/>
           <a:chOff x="37652894" y="695690"/>
           <a:chExt cx="3190115" cy="3644785"/>
         </a:xfrm>
@@ -23674,8 +23674,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="62933146" y="1208317"/>
-          <a:ext cx="3551996" cy="6272061"/>
+          <a:off x="63110759" y="1211118"/>
+          <a:ext cx="3563202" cy="6323048"/>
           <a:chOff x="59141720" y="969818"/>
           <a:chExt cx="3164884" cy="3644791"/>
         </a:xfrm>
@@ -27156,8 +27156,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9941315" y="1094054"/>
-          <a:ext cx="3549743" cy="6374352"/>
+          <a:off x="9954202" y="1094054"/>
+          <a:ext cx="3560949" cy="6428140"/>
           <a:chOff x="8657441" y="675408"/>
           <a:chExt cx="3193556" cy="3763407"/>
         </a:xfrm>
@@ -28058,8 +28058,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31802324" y="25165237"/>
-          <a:ext cx="3522633" cy="4935612"/>
+          <a:off x="31886928" y="25429136"/>
+          <a:ext cx="3525995" cy="4994442"/>
           <a:chOff x="27945820" y="22949647"/>
           <a:chExt cx="3141633" cy="3755818"/>
         </a:xfrm>
@@ -28807,8 +28807,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31763821" y="8202706"/>
-          <a:ext cx="3544322" cy="4937467"/>
+          <a:off x="31848425" y="8264899"/>
+          <a:ext cx="3547684" cy="4996298"/>
           <a:chOff x="27936265" y="9681882"/>
           <a:chExt cx="3176022" cy="3757675"/>
         </a:xfrm>
@@ -29662,8 +29662,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31821284" y="1217842"/>
-          <a:ext cx="3539906" cy="6281586"/>
+          <a:off x="31905888" y="1220643"/>
+          <a:ext cx="3543268" cy="6332573"/>
           <a:chOff x="46386774" y="6092825"/>
           <a:chExt cx="3184493" cy="3811623"/>
         </a:xfrm>
@@ -31030,8 +31030,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31786246" y="19464833"/>
-          <a:ext cx="3606750" cy="4937367"/>
+          <a:off x="31870850" y="19661496"/>
+          <a:ext cx="3610112" cy="4996198"/>
           <a:chOff x="27961865" y="13634599"/>
           <a:chExt cx="3228925" cy="3767099"/>
         </a:xfrm>
@@ -41480,8 +41480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E4BCCA-608F-4C56-8910-30F772A13230}">
   <dimension ref="B2:AM106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="AU22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BB37" sqref="BB37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Creating journal entry screens with grid view
</commit_message>
<xml_diff>
--- a/Documentation/Project Overview.xlsx
+++ b/Documentation/Project Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Working-Space\Ship-Journal\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB76030D-F10E-4F87-8286-A648CF716656}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B954E405-2D94-4E9D-8C77-3BA532B96273}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="2" xr2:uid="{A0F38D15-187F-4603-A4E4-C66A63208D0B}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="57">
   <si>
     <t>Version</t>
   </si>
@@ -218,6 +218,10 @@
   </si>
   <si>
     <t>Insert the logo of the National Research and Development Agency, Fisheries Research and Education Agency, in the top right corner of the first level</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -18268,12 +18272,12 @@
                     <a:lstStyle/>
                     <a:p>
                       <a:r>
-                        <a:rPr lang="ja-JP" altLang="en-US" sz="1400" b="1">
+                        <a:rPr lang="en-US" altLang="ja-JP" sz="1400" b="1">
                           <a:solidFill>
                             <a:sysClr val="windowText" lastClr="000000"/>
                           </a:solidFill>
                         </a:rPr>
-                        <a:t>コメント</a:t>
+                        <a:t>Comment</a:t>
                       </a:r>
                       <a:endParaRPr lang="en-US" sz="1400" b="1">
                         <a:solidFill>
@@ -19191,8 +19195,8 @@
                 <a:p>
                   <a:pPr algn="ctr"/>
                   <a:r>
-                    <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
-                    <a:t>項目</a:t>
+                    <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
+                    <a:t>Item</a:t>
                   </a:r>
                   <a:endParaRPr lang="en-US" sz="1100" b="1"/>
                 </a:p>
@@ -19242,8 +19246,8 @@
                 <a:p>
                   <a:pPr algn="ctr"/>
                   <a:r>
-                    <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
-                    <a:t>数値</a:t>
+                    <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
+                    <a:t>Qty</a:t>
                   </a:r>
                   <a:endParaRPr lang="en-US" sz="1100" b="1"/>
                 </a:p>
@@ -19997,12 +20001,12 @@
                     <a:lstStyle/>
                     <a:p>
                       <a:r>
-                        <a:rPr lang="ja-JP" altLang="en-US" sz="1400" b="1">
+                        <a:rPr lang="en-US" altLang="ja-JP" sz="1400" b="1">
                           <a:solidFill>
                             <a:sysClr val="windowText" lastClr="000000"/>
                           </a:solidFill>
                         </a:rPr>
-                        <a:t>コメント</a:t>
+                        <a:t>Comment</a:t>
                       </a:r>
                       <a:endParaRPr lang="en-US" sz="1400" b="1">
                         <a:solidFill>
@@ -20920,8 +20924,8 @@
                 <a:p>
                   <a:pPr algn="ctr"/>
                   <a:r>
-                    <a:rPr lang="ja-JP" altLang="en-US" sz="1100" b="1"/>
-                    <a:t>項目</a:t>
+                    <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="1"/>
+                    <a:t>Item</a:t>
                   </a:r>
                   <a:endParaRPr lang="en-US" sz="1100" b="1"/>
                 </a:p>
@@ -21726,12 +21730,12 @@
                     <a:lstStyle/>
                     <a:p>
                       <a:r>
-                        <a:rPr lang="ja-JP" altLang="en-US" sz="1400" b="1">
+                        <a:rPr lang="en-US" altLang="ja-JP" sz="1400" b="1">
                           <a:solidFill>
                             <a:sysClr val="windowText" lastClr="000000"/>
                           </a:solidFill>
                         </a:rPr>
-                        <a:t>コメント</a:t>
+                        <a:t>Comment</a:t>
                       </a:r>
                       <a:endParaRPr lang="en-US" sz="1400" b="1">
                         <a:solidFill>
@@ -41407,7 +41411,7 @@
   <dimension ref="F2:AH3"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="20.25" x14ac:dyDescent="0.35"/>
@@ -41472,10 +41476,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E4BCCA-608F-4C56-8910-30F772A13230}">
-  <dimension ref="B2:AM106"/>
+  <dimension ref="A2:BB106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE92" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT116" sqref="AT116"/>
+    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -41497,12 +41501,12 @@
     <col min="40" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.4">
       <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="2:39" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:54" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
@@ -41528,7 +41532,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>25</v>
       </c>
@@ -41539,7 +41543,7 @@
         <v>45567</v>
       </c>
     </row>
-    <row r="5" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.4">
       <c r="B5" s="10" t="s">
         <v>27</v>
       </c>
@@ -41550,7 +41554,7 @@
         <v>45567</v>
       </c>
     </row>
-    <row r="6" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.4">
       <c r="B6" s="10" t="s">
         <v>29</v>
       </c>
@@ -41561,7 +41565,7 @@
         <v>45567</v>
       </c>
     </row>
-    <row r="7" spans="2:39" ht="37.5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:54" ht="37.5" x14ac:dyDescent="0.4">
       <c r="B7" s="10" t="s">
         <v>31</v>
       </c>
@@ -41572,7 +41576,7 @@
         <v>45567</v>
       </c>
     </row>
-    <row r="8" spans="2:39" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:54" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="10" t="s">
         <v>33</v>
       </c>
@@ -41583,7 +41587,7 @@
         <v>45568</v>
       </c>
     </row>
-    <row r="9" spans="2:39" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:54" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="10" t="s">
         <v>35</v>
       </c>
@@ -41594,7 +41598,10 @@
         <v>45574</v>
       </c>
     </row>
-    <row r="10" spans="2:39" ht="73.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:54" ht="73.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="B10" s="10" t="s">
         <v>37</v>
       </c>
@@ -41604,8 +41611,11 @@
       <c r="D10" s="13">
         <v>45574</v>
       </c>
+      <c r="BB10" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="11" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.4">
       <c r="B11" s="10" t="s">
         <v>39</v>
       </c>
@@ -41616,7 +41626,7 @@
         <v>45574</v>
       </c>
     </row>
-    <row r="12" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.4">
       <c r="B12" s="10" t="s">
         <v>41</v>
       </c>
@@ -41627,22 +41637,22 @@
         <v>45574</v>
       </c>
     </row>
-    <row r="13" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.4">
       <c r="B13" s="10"/>
       <c r="C13" s="12"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.4">
       <c r="B14" s="10"/>
       <c r="C14" s="12"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.4">
       <c r="B15" s="10"/>
       <c r="C15" s="12"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.4">
       <c r="B16" s="10"/>
       <c r="C16" s="12"/>
       <c r="D16" s="10"/>

</xml_diff>

<commit_message>
Update code for FO remaining screen
</commit_message>
<xml_diff>
--- a/Documentation/Project Overview.xlsx
+++ b/Documentation/Project Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Working-Space\Ship-Journal\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B954E405-2D94-4E9D-8C77-3BA532B96273}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E1BBE2-19ED-48F1-A592-E9A66178CA87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="2" xr2:uid="{A0F38D15-187F-4603-A4E4-C66A63208D0B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" activeTab="1" xr2:uid="{A0F38D15-187F-4603-A4E4-C66A63208D0B}"/>
   </bookViews>
   <sheets>
     <sheet name=" Revision History" sheetId="1" r:id="rId1"/>
@@ -4058,15 +4058,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>451224</xdr:colOff>
+      <xdr:colOff>271930</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>7841</xdr:rowOff>
+      <xdr:rowOff>19047</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>228787</xdr:colOff>
+      <xdr:colOff>49493</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>131106</xdr:rowOff>
+      <xdr:rowOff>142312</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4079,14 +4079,12 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
-          <a:stCxn id="230" idx="3"/>
-          <a:endCxn id="151" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7452099" y="1598516"/>
-          <a:ext cx="1796863" cy="9381565"/>
+          <a:off x="7264401" y="1610282"/>
+          <a:ext cx="1794621" cy="9401736"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector4">
           <a:avLst>
@@ -4123,14 +4121,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>456079</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>47864</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>7841</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>228787</xdr:colOff>
+      <xdr:colOff>324037</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>98048</xdr:rowOff>
     </xdr:to>
@@ -4145,14 +4143,12 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
-          <a:stCxn id="235" idx="3"/>
-          <a:endCxn id="151" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7018804" y="1436591"/>
-          <a:ext cx="1792008" cy="9377082"/>
+          <a:off x="7531793" y="1599877"/>
+          <a:ext cx="1786565" cy="10173100"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector4">
           <a:avLst>
@@ -4190,15 +4186,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>459068</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>7841</xdr:rowOff>
+      <xdr:colOff>440018</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>217391</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>228787</xdr:colOff>
+      <xdr:colOff>209737</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>93566</xdr:rowOff>
+      <xdr:rowOff>45941</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4211,14 +4207,12 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
-          <a:stCxn id="236" idx="3"/>
-          <a:endCxn id="151" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7021793" y="1436591"/>
-          <a:ext cx="1789019" cy="10086975"/>
+          <a:off x="7440893" y="1550891"/>
+          <a:ext cx="1789019" cy="10887075"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector4">
           <a:avLst>
@@ -5890,16 +5884,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>1494</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>412749</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>7841</xdr:rowOff>
+      <xdr:rowOff>86282</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>228787</xdr:colOff>
+      <xdr:colOff>135778</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>74890</xdr:rowOff>
+      <xdr:rowOff>153331</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5912,14 +5906,12 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
-          <a:stCxn id="243" idx="3"/>
-          <a:endCxn id="151" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7069044" y="1436591"/>
-          <a:ext cx="1741768" cy="10782674"/>
+          <a:off x="7413624" y="1676957"/>
+          <a:ext cx="1742329" cy="11639924"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector4">
           <a:avLst>
@@ -9663,8 +9655,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="26289000" y="1187824"/>
-          <a:ext cx="3549743" cy="6206934"/>
+          <a:off x="26365200" y="1181100"/>
+          <a:ext cx="3560949" cy="6121770"/>
           <a:chOff x="8189026" y="682665"/>
           <a:chExt cx="3183247" cy="3803567"/>
         </a:xfrm>
@@ -10136,8 +10128,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="20820529" y="1188772"/>
-          <a:ext cx="3549744" cy="6205985"/>
+          <a:off x="20878800" y="1182048"/>
+          <a:ext cx="3560949" cy="6120821"/>
           <a:chOff x="18340779" y="725723"/>
           <a:chExt cx="3183248" cy="3806675"/>
         </a:xfrm>
@@ -10802,8 +10794,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="47398378" y="7819221"/>
-          <a:ext cx="3653731" cy="4946585"/>
+          <a:off x="47553019" y="7713886"/>
+          <a:ext cx="3667178" cy="4805391"/>
           <a:chOff x="27944990" y="737920"/>
           <a:chExt cx="3196481" cy="3898206"/>
         </a:xfrm>
@@ -12381,8 +12373,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="42879211" y="7830649"/>
-          <a:ext cx="3555087" cy="4928858"/>
+          <a:off x="43020405" y="7725314"/>
+          <a:ext cx="3566293" cy="4787664"/>
           <a:chOff x="27963633" y="5221724"/>
           <a:chExt cx="3181788" cy="3896347"/>
         </a:xfrm>
@@ -13829,8 +13821,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="15359202" y="1206461"/>
-          <a:ext cx="3546560" cy="6254409"/>
+          <a:off x="15399543" y="1199737"/>
+          <a:ext cx="3557766" cy="6162521"/>
           <a:chOff x="13431899" y="760845"/>
           <a:chExt cx="3156281" cy="3890158"/>
         </a:xfrm>
@@ -14453,8 +14445,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31798362" y="13892122"/>
-          <a:ext cx="3616295" cy="4950991"/>
+          <a:off x="31892491" y="13611975"/>
+          <a:ext cx="3638707" cy="4809797"/>
           <a:chOff x="27998557" y="14473052"/>
           <a:chExt cx="3240382" cy="3893177"/>
         </a:xfrm>
@@ -16354,8 +16346,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="42836052" y="1190787"/>
-          <a:ext cx="3577227" cy="6272055"/>
+          <a:off x="42977246" y="1184063"/>
+          <a:ext cx="3588433" cy="6180167"/>
           <a:chOff x="37652894" y="695690"/>
           <a:chExt cx="3186940" cy="3641610"/>
         </a:xfrm>
@@ -18088,8 +18080,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="47387517" y="1187824"/>
-          <a:ext cx="3661005" cy="6275236"/>
+          <a:off x="47542158" y="1181100"/>
+          <a:ext cx="3674452" cy="6183348"/>
           <a:chOff x="37652894" y="695690"/>
           <a:chExt cx="3190115" cy="3644785"/>
         </a:xfrm>
@@ -19817,8 +19809,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="52253029" y="1187824"/>
-          <a:ext cx="3580409" cy="6272061"/>
+          <a:off x="52425600" y="1181100"/>
+          <a:ext cx="3591614" cy="6180173"/>
           <a:chOff x="37652894" y="695690"/>
           <a:chExt cx="3190115" cy="3644785"/>
         </a:xfrm>
@@ -21546,8 +21538,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="57037941" y="1187824"/>
-          <a:ext cx="3577233" cy="6275236"/>
+          <a:off x="57226200" y="1181100"/>
+          <a:ext cx="3588439" cy="6183348"/>
           <a:chOff x="37652894" y="695690"/>
           <a:chExt cx="3190115" cy="3644785"/>
         </a:xfrm>
@@ -23675,8 +23667,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="62933146" y="1208317"/>
-          <a:ext cx="3551996" cy="6272061"/>
+          <a:off x="63139334" y="1201593"/>
+          <a:ext cx="3563202" cy="6180173"/>
           <a:chOff x="59141720" y="969818"/>
           <a:chExt cx="3164884" cy="3644791"/>
         </a:xfrm>
@@ -27157,8 +27149,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9941315" y="1094054"/>
-          <a:ext cx="3549743" cy="6374352"/>
+          <a:off x="9963727" y="1094054"/>
+          <a:ext cx="3560949" cy="6275740"/>
           <a:chOff x="8657441" y="675408"/>
           <a:chExt cx="3193556" cy="3763407"/>
         </a:xfrm>
@@ -28059,8 +28051,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31802324" y="25165237"/>
-          <a:ext cx="3522633" cy="4935612"/>
+          <a:off x="31896453" y="24562361"/>
+          <a:ext cx="3545045" cy="4794417"/>
           <a:chOff x="27945820" y="22949647"/>
           <a:chExt cx="3141633" cy="3755818"/>
         </a:xfrm>
@@ -28808,8 +28800,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31763821" y="8202706"/>
-          <a:ext cx="3544322" cy="4937467"/>
+          <a:off x="31857950" y="8083924"/>
+          <a:ext cx="3566734" cy="4796273"/>
           <a:chOff x="27936265" y="9681882"/>
           <a:chExt cx="3176022" cy="3757675"/>
         </a:xfrm>
@@ -29663,8 +29655,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31821284" y="1217842"/>
-          <a:ext cx="3539906" cy="6281586"/>
+          <a:off x="31915413" y="1211118"/>
+          <a:ext cx="3562318" cy="6189698"/>
           <a:chOff x="46386774" y="6092825"/>
           <a:chExt cx="3184493" cy="3811623"/>
         </a:xfrm>
@@ -31031,8 +31023,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="31786246" y="19464833"/>
-          <a:ext cx="3606750" cy="4937367"/>
+          <a:off x="31880375" y="19023321"/>
+          <a:ext cx="3629162" cy="4796173"/>
           <a:chOff x="27961865" y="13634599"/>
           <a:chExt cx="3228925" cy="3767099"/>
         </a:xfrm>
@@ -32185,16 +32177,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>533282</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>17880</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>40223</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>96321</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>40642</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>53062</xdr:rowOff>
+      <xdr:colOff>231142</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>131504</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -32209,7 +32201,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29556517" y="4175262"/>
+          <a:off x="29747017" y="4018380"/>
           <a:ext cx="2241596" cy="4271006"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
@@ -32672,8 +32664,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="15633011" y="953294"/>
-          <a:ext cx="3524363" cy="6161268"/>
+          <a:off x="15689040" y="926400"/>
+          <a:ext cx="3535569" cy="6094033"/>
           <a:chOff x="13590364" y="26574050"/>
           <a:chExt cx="3202194" cy="4011233"/>
         </a:xfrm>
@@ -33319,8 +33311,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="21083782" y="948551"/>
-          <a:ext cx="3502949" cy="6026582"/>
+          <a:off x="21157741" y="921657"/>
+          <a:ext cx="3514155" cy="5966070"/>
           <a:chOff x="13435075" y="760845"/>
           <a:chExt cx="3153104" cy="3890158"/>
         </a:xfrm>
@@ -34102,8 +34094,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="26505064" y="941666"/>
-          <a:ext cx="3554644" cy="6097855"/>
+          <a:off x="26596952" y="914772"/>
+          <a:ext cx="3565850" cy="6037343"/>
           <a:chOff x="18406733" y="715323"/>
           <a:chExt cx="3195282" cy="3708174"/>
         </a:xfrm>
@@ -34477,8 +34469,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="26510983" y="7502679"/>
-          <a:ext cx="3551469" cy="4941573"/>
+          <a:off x="26602871" y="7401826"/>
+          <a:ext cx="3562675" cy="4800379"/>
           <a:chOff x="18406733" y="715323"/>
           <a:chExt cx="3195282" cy="3708174"/>
         </a:xfrm>
@@ -35058,8 +35050,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="21095353" y="7563691"/>
-          <a:ext cx="3502949" cy="4818215"/>
+          <a:off x="21169312" y="7462838"/>
+          <a:ext cx="3514155" cy="4677021"/>
           <a:chOff x="13435075" y="760845"/>
           <a:chExt cx="3153104" cy="3890158"/>
         </a:xfrm>
@@ -35500,8 +35492,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10151794" y="913790"/>
-          <a:ext cx="3538981" cy="6199323"/>
+          <a:off x="10189894" y="893619"/>
+          <a:ext cx="3550187" cy="6125365"/>
           <a:chOff x="8657441" y="675408"/>
           <a:chExt cx="3193556" cy="3763407"/>
         </a:xfrm>
@@ -36553,8 +36545,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="15348015" y="959931"/>
-          <a:ext cx="3545113" cy="6153481"/>
+          <a:off x="15399562" y="933037"/>
+          <a:ext cx="3556319" cy="6086246"/>
           <a:chOff x="13508623" y="726208"/>
           <a:chExt cx="3185751" cy="3708171"/>
         </a:xfrm>
@@ -37130,8 +37122,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="20822699" y="944236"/>
-          <a:ext cx="3551469" cy="6161469"/>
+          <a:off x="20892175" y="917342"/>
+          <a:ext cx="3562675" cy="6094234"/>
           <a:chOff x="18406733" y="715323"/>
           <a:chExt cx="3195282" cy="3708174"/>
         </a:xfrm>
@@ -37651,8 +37643,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="20812823" y="9460225"/>
-          <a:ext cx="3551469" cy="4874327"/>
+          <a:off x="20882299" y="9298860"/>
+          <a:ext cx="3562675" cy="4739857"/>
           <a:chOff x="18406733" y="715323"/>
           <a:chExt cx="3195282" cy="3708174"/>
         </a:xfrm>
@@ -38815,8 +38807,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="20755447" y="15150765"/>
-          <a:ext cx="3603587" cy="4863385"/>
+          <a:off x="20822682" y="14828036"/>
+          <a:ext cx="3617034" cy="4728914"/>
           <a:chOff x="18404114" y="10599964"/>
           <a:chExt cx="3237194" cy="3635565"/>
         </a:xfrm>
@@ -40337,8 +40329,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9926811" y="1006155"/>
-          <a:ext cx="3546568" cy="6207863"/>
+          <a:off x="9960429" y="979261"/>
+          <a:ext cx="3557774" cy="6140628"/>
           <a:chOff x="8657441" y="675408"/>
           <a:chExt cx="3193556" cy="3763407"/>
         </a:xfrm>
@@ -41309,7 +41301,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.4"/>
@@ -41410,8 +41402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD51CE1-DE9E-4F8D-A2FF-EE74C34B2238}">
   <dimension ref="F2:AH3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="20.25" x14ac:dyDescent="0.35"/>
@@ -41478,8 +41470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E4BCCA-608F-4C56-8910-30F772A13230}">
   <dimension ref="A2:BB106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="BC55" sqref="BC55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -41687,7 +41679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4C208A-A99A-4A43-BB1B-AD32838C9000}">
   <dimension ref="B2:AM17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -41876,7 +41868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65059E32-4F8B-40EB-A291-F3015047563B}">
   <dimension ref="B2:AM17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>

</xml_diff>